<commit_message>
Ajout Rapport et dernières modifications
</commit_message>
<xml_diff>
--- a/Matrice Implication PROGAV.xlsx
+++ b/Matrice Implication PROGAV.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3DE855-40F5-4A6F-B083-77198260C913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD718F08-0138-4502-B18A-21F732C79BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>n°</t>
   </si>
@@ -118,7 +118,7 @@
     <t>40 / 60</t>
   </si>
   <si>
-    <t>60 / 40</t>
+    <t>65 / 35</t>
   </si>
 </sst>
 </file>
@@ -462,6 +462,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -494,10 +498,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,38 +797,38 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="2:5" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="26"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
@@ -848,13 +848,13 @@
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="20" t="s">
         <v>28</v>
       </c>
     </row>
@@ -863,13 +863,13 @@
         <f>1+B7</f>
         <v>2</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -878,39 +878,39 @@
         <f t="shared" ref="B9:B21" si="0">1+B8</f>
         <v>3</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="20"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -919,26 +919,26 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="20" t="s">
         <v>27</v>
       </c>
     </row>
@@ -947,26 +947,26 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="20" t="s">
         <v>27</v>
       </c>
     </row>
@@ -975,13 +975,13 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="20" t="s">
         <v>27</v>
       </c>
     </row>
@@ -990,52 +990,41 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>27</v>
-      </c>
+      <c r="D17" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="31"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
       <c r="E19" s="17"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
       <c r="E20" s="17"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="4">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
       <c r="E21" s="18"/>

</xml_diff>